<commit_message>
Implemented BFS with backtracking to solve sudoku
</commit_message>
<xml_diff>
--- a/Sudoku/sudoku3.xlsx
+++ b/Sudoku/sudoku3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Sudoku-Solver\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elon\Desktop\AI-2023-2024-GR10\Sudoku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C4E00D4-3EBB-4EF4-A3CA-F07C303AF212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{041843DB-9986-4C4D-A47B-490D06CC0DAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>Sudoku</t>
-  </si>
-  <si>
-    <t>I</t>
   </si>
 </sst>
 </file>
@@ -529,15 +526,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="24" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -550,10 +547,8 @@
       <c r="H1" s="10"/>
       <c r="I1" s="10"/>
     </row>
-    <row r="2" spans="1:10" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
+    <row r="2" spans="1:9" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
       <c r="D2" s="1">
@@ -569,7 +564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -580,7 +575,7 @@
       <c r="H3" s="5"/>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="1:10" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -593,7 +588,7 @@
       <c r="H4" s="8"/>
       <c r="I4" s="9"/>
     </row>
-    <row r="5" spans="1:10" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>8</v>
       </c>
@@ -606,7 +601,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:10" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>
@@ -619,7 +614,7 @@
       <c r="H6" s="5"/>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:10" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="7"/>
       <c r="B7" s="8"/>
       <c r="C7" s="9"/>
@@ -632,7 +627,7 @@
       </c>
       <c r="I7" s="9"/>
     </row>
-    <row r="8" spans="1:10" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="3"/>
@@ -644,11 +639,8 @@
       <c r="I8" s="3">
         <v>4</v>
       </c>
-      <c r="J8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:9" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="C9" s="6"/>
@@ -661,7 +653,7 @@
       </c>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:10" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -676,7 +668,7 @@
       <c r="H10" s="8"/>
       <c r="I10" s="9"/>
     </row>
-    <row r="11" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>

</xml_diff>